<commit_message>
Finished Field Download component.
</commit_message>
<xml_diff>
--- a/static/fields/foodevent_reference.xlsx
+++ b/static/fields/foodevent_reference.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36480" yWindow="0" windowWidth="30720" windowHeight="20060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="foodevent_field_reference_list." sheetId="1" r:id="rId1"/>
+    <sheet name="food_event_fields" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -748,7 +748,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -760,7 +760,7 @@
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -774,7 +774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -788,7 +788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -802,7 +802,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -816,7 +816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="90">
+    <row r="5" spans="1:4" ht="90">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -830,7 +830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -844,7 +844,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="135">
+    <row r="7" spans="1:4" ht="135">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -858,7 +858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="240">
+    <row r="8" spans="1:4" ht="240">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -872,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="240">
+    <row r="9" spans="1:4" ht="240">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -886,7 +886,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" ht="409">
+    <row r="10" spans="1:4" ht="409">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" ht="270">
+    <row r="11" spans="1:4" ht="270">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -914,7 +914,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="3" customFormat="1" ht="409">
+    <row r="12" spans="1:4" ht="409">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>